<commit_message>
Tasks solved at 08.02.2022
Tasks solved at 08.02.2022
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,15 +65,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -376,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +406,9 @@
       <c r="B3" s="1">
         <v>44605</v>
       </c>
+      <c r="C3" s="1">
+        <v>44600</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">

</xml_diff>

<commit_message>
Tasks solved at 10.02.2022.
Tasks solved at 10.02.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1305" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,6 +417,9 @@
       <c r="B4" s="1">
         <v>44612</v>
       </c>
+      <c r="C4" s="1">
+        <v>44602</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>

<commit_message>
Tasks solved at 15.02.2022.
Tasks solved at 15.02.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,6 +428,9 @@
       <c r="B5" s="1">
         <v>44619</v>
       </c>
+      <c r="C5" s="1">
+        <v>44607</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>

<commit_message>
Tasks solved at 27.02.2022.
Tasks solved at 27.02.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2505" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="3105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +439,9 @@
       <c r="B6" s="1">
         <v>44626</v>
       </c>
+      <c r="C6" s="1">
+        <v>44619</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">

</xml_diff>

<commit_message>
Tasks solved at 28.02.2022.
Tasks solved at 28.02.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="3705" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +450,9 @@
       <c r="B7" s="1">
         <v>44633</v>
       </c>
+      <c r="C7" s="1">
+        <v>44620</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">

</xml_diff>

<commit_message>
Tasks solved on this week.
Tasks solved on this week.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="3705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="4305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +461,9 @@
       <c r="B8" s="1">
         <v>44640</v>
       </c>
+      <c r="C8" s="1">
+        <v>44622</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">

</xml_diff>

<commit_message>
Tasks solved at 05.04.2022.
Tasks solved at 05.04.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4305" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="4905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +472,9 @@
       <c r="B9" s="1">
         <v>44647</v>
       </c>
+      <c r="C9" s="1">
+        <v>44656</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">

</xml_diff>

<commit_message>
Tasks solved at 11.04.2022.
Tasks solved at 11.04.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="5505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,6 +483,9 @@
       <c r="B10" s="1">
         <v>44654</v>
       </c>
+      <c r="C10" s="1">
+        <v>44662</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">

</xml_diff>

<commit_message>
Tasks solved at 21.04.2022.
Tasks solved at 21.04.2022.
</commit_message>
<xml_diff>
--- a/3 Months Preparation Kit/План.xlsx
+++ b/3 Months Preparation Kit/План.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="5505" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="6105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,6 +494,9 @@
       <c r="B11" s="1">
         <v>44661</v>
       </c>
+      <c r="C11" s="1">
+        <v>44672</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">

</xml_diff>